<commit_message>
debugging ExcelDoc EffectiveDate setter.
</commit_message>
<xml_diff>
--- a/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev1.xlsx
+++ b/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev1.xlsx
@@ -604,133 +604,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:E12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.85546875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader xml:space="preserve">&amp;L&amp;G&amp;C&amp;"Arial,Regular"&amp;10DOCUMENT NAME: &amp;"Arial,Bold"Document Control Index (F-001B)&amp;R&amp;"Arial,Regular"&amp;10&amp;K000000Effective Date: 2018-11-26 
-Revision: 2 </oddHeader>
-    <oddFooter>&amp;R&amp;"Arial,Normal"&amp;10Page &amp;P of &amp;N</oddFooter>
-  </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:pageSetUpPr fitToPage="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E12"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <x:selection activeCell="E6" sqref="E6"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <x:cols>
+    <x:col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
+    <x:col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
+    <x:col min="3" max="3" width="59.85546875" style="1" customWidth="1"/>
+    <x:col min="4" max="4" width="9.28515625" style="2" customWidth="1"/>
+    <x:col min="5" max="5" width="13" style="7" customWidth="1"/>
+    <x:col min="6" max="6" width="14" style="1" customWidth="1"/>
+    <x:col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <x:col min="8" max="16384" width="10.85546875" style="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <x:c r="A1" s="12" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B1" s="13"/>
+      <x:c r="C1" s="3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="D1" s="4" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="E1" s="5" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A2" s="10"/>
+      <x:c r="B2" s="10"/>
+      <x:c r="C2" s="10"/>
+      <x:c r="D2" s="11"/>
+      <x:c r="E2" s="11"/>
+    </x:row>
+    <x:row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A3" s="10"/>
+      <x:c r="B3" s="10"/>
+      <x:c r="C3" s="10"/>
+      <x:c r="D3" s="11"/>
+      <x:c r="E3" s="11"/>
+    </x:row>
+    <x:row r="4" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A4" s="10"/>
+      <x:c r="B4" s="10"/>
+      <x:c r="C4" s="10"/>
+      <x:c r="D4" s="11"/>
+      <x:c r="E4" s="11"/>
+    </x:row>
+    <x:row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A5" s="10"/>
+      <x:c r="B5" s="10"/>
+      <x:c r="C5" s="10"/>
+      <x:c r="D5" s="11"/>
+      <x:c r="E5" s="11"/>
+    </x:row>
+    <x:row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A6" s="10"/>
+      <x:c r="B6" s="10"/>
+      <x:c r="C6" s="10"/>
+      <x:c r="D6" s="11"/>
+      <x:c r="E6" s="11"/>
+    </x:row>
+    <x:row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A7" s="10"/>
+      <x:c r="B7" s="10"/>
+      <x:c r="C7" s="10"/>
+      <x:c r="D7" s="11"/>
+      <x:c r="E7" s="11"/>
+    </x:row>
+    <x:row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A8" s="10"/>
+      <x:c r="B8" s="10"/>
+      <x:c r="C8" s="10"/>
+      <x:c r="D8" s="11"/>
+      <x:c r="E8" s="11"/>
+    </x:row>
+    <x:row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A9" s="10"/>
+      <x:c r="B9" s="10"/>
+      <x:c r="C9" s="10"/>
+      <x:c r="D9" s="11"/>
+      <x:c r="E9" s="11"/>
+    </x:row>
+    <x:row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A10" s="10"/>
+      <x:c r="B10" s="10"/>
+      <x:c r="C10" s="10"/>
+      <x:c r="D10" s="11"/>
+      <x:c r="E10" s="11"/>
+    </x:row>
+    <x:row r="11" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A11" s="10"/>
+      <x:c r="B11" s="10"/>
+      <x:c r="C11" s="10"/>
+      <x:c r="D11" s="11"/>
+      <x:c r="E11" s="11"/>
+    </x:row>
+    <x:row r="12" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <x:c r="A12" s="10"/>
+      <x:c r="B12" s="10"/>
+      <x:c r="C12" s="10"/>
+      <x:c r="D12" s="11"/>
+      <x:c r="E12" s="11"/>
+    </x:row>
+  </x:sheetData>
+  <x:mergeCells count="1">
+    <x:mergeCell ref="A1:B1"/>
+  </x:mergeCells>
+  <x:phoneticPr fontId="4" type="noConversion"/>
+  <x:printOptions horizontalCentered="1"/>
+  <x:pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <x:pageSetup scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <x:headerFooter alignWithMargins="0">
+    <x:oddHeader xml:space="preserve">&amp;L&amp;G&amp;C&amp;"Arial,Regular"&amp;10DOCUMENT NAME: &amp;"Arial,Bold"Document Control Index (F-001B)&amp;R&amp;"Arial,Regular"&amp;10&amp;K000000Effective Date: 2018-11-26 
+Revision: 2 </x:oddHeader>
+    <x:oddFooter>&amp;R&amp;"Arial,Normal"&amp;10Page &amp;P of &amp;N</x:oddFooter>
+  </x:headerFooter>
+  <x:legacyDrawingHF r:id="rId2"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
broke the QmsDoc.Test fixture files...will replace tomorrow.
</commit_message>
<xml_diff>
--- a/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev1.xlsx
+++ b/QmsHero/QmsDoc.Test/Fixtures/Active QMS Documents/SOP-001 Quality Manual Documents/F-001B Document Control Index Rev1.xlsx
@@ -726,11 +726,6 @@
   <x:printOptions horizontalCentered="1"/>
   <x:pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <x:pageSetup scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
-  <x:headerFooter alignWithMargins="0">
-    <x:oddHeader xml:space="preserve">&amp;L&amp;G&amp;C&amp;"Arial,Regular"&amp;10DOCUMENT NAME: &amp;"Arial,Bold"Document Control Index (F-001B)&amp;R&amp;"Arial,Regular"&amp;10&amp;K000000Effective Date: 2018-11-26 
-Revision: 2 </x:oddHeader>
-    <x:oddFooter>&amp;R&amp;"Arial,Normal"&amp;10Page &amp;P of &amp;N</x:oddFooter>
-  </x:headerFooter>
   <x:legacyDrawingHF r:id="rId2"/>
 </x:worksheet>
 </file>
</xml_diff>